<commit_message>
Added CSV_Manager file which will scrape a website for all related product information and eventually create a CSV file containing an organized and easy to read format of that information
</commit_message>
<xml_diff>
--- a/MLJTPCX1GXDCF_catalog-2025-06-10-1510.xlsx
+++ b/MLJTPCX1GXDCF_catalog-2025-06-10-1510.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecd247867560937e/Desktop/WebDevelopment/ProjectForShawn/csv_organizer/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ecd247867560937e/Desktop/WebDevelopment/ProjectForShawn/InventoryManager/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_9B634F2A3846757CB63510CDC567D37630DD1D7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E6233125-745E-46CB-BB73-7BAF4CF85251}"/>
+  <xr:revisionPtr revIDLastSave="17" documentId="11_9B634F2A3846757CB63510CDC567D37630DD1D7A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5386EC5A-8916-48BC-BBDA-663478A45763}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="6228" yWindow="1416" windowWidth="27648" windowHeight="16224" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2304" yWindow="1056" windowWidth="26532" windowHeight="16224" tabRatio="204" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -1800,6 +1800,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2126,7 +2130,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:AD95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2143,7 +2147,8 @@
     <col min="11" max="11" width="23.23046875" customWidth="1"/>
     <col min="12" max="14" width="9.4609375"/>
     <col min="15" max="15" width="9.4609375" style="1"/>
-    <col min="16" max="22" width="9.4609375"/>
+    <col min="16" max="16" width="19.3828125" customWidth="1"/>
+    <col min="17" max="22" width="9.4609375"/>
     <col min="23" max="23" width="26.07421875" customWidth="1"/>
     <col min="24" max="24" width="9.4609375" style="1"/>
     <col min="25" max="30" width="9.4609375"/>

</xml_diff>